<commit_message>
Amended a couple of entries in the risk assessment
</commit_message>
<xml_diff>
--- a/Documentation/risk-assessment-template.xlsx
+++ b/Documentation/risk-assessment-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dssan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dssan\eclipse-workspace\QASpringToDoListProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3924DD48-E411-4473-9BFC-90D833674C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44109EC7-2768-4F69-AA25-67347EC21E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,9 +120,6 @@
     <t xml:space="preserve">My wrists could be aching </t>
   </si>
   <si>
-    <t xml:space="preserve">Ensure I move wrists about </t>
-  </si>
-  <si>
     <t>To keep my wrists safe for the future</t>
   </si>
   <si>
@@ -183,12 +180,6 @@
     <t>Maintain communication where possible, focus on any opportunities to progress available</t>
   </si>
   <si>
-    <t>Global Pandemic</t>
-  </si>
-  <si>
-    <t>Get vaccinated</t>
-  </si>
-  <si>
     <t>Super Unlikely</t>
   </si>
   <si>
@@ -198,7 +189,16 @@
     <t>Just keep going, one way or another</t>
   </si>
   <si>
-    <t>A virus could spread across the entire planet killing millions and infecting hundreds of millions</t>
+    <t>Ensure I move wrists about and wear wrist supports</t>
+  </si>
+  <si>
+    <t>Possible World War 3</t>
+  </si>
+  <si>
+    <t>A large nation could invade its neighbour with the potential to spark a nuclear conflict between world superpowers</t>
+  </si>
+  <si>
+    <t>Read "When the Wind Blows" to relax</t>
   </si>
 </sst>
 </file>
@@ -873,8 +873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -1043,10 +1043,10 @@
         <v>27</v>
       </c>
       <c r="D12" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="27" t="s">
         <v>28</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>29</v>
       </c>
       <c r="F12" s="28" t="s">
         <v>13</v>
@@ -1058,16 +1058,16 @@
     </row>
     <row r="13" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="D13" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="19" t="s">
         <v>31</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>32</v>
       </c>
       <c r="F13" s="20" t="s">
         <v>10</v>
@@ -1079,16 +1079,16 @@
     </row>
     <row r="14" spans="2:8" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="D14" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="E14" s="19" t="s">
         <v>36</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>37</v>
       </c>
       <c r="F14" s="20" t="s">
         <v>6</v>
@@ -1100,16 +1100,16 @@
     </row>
     <row r="15" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B15" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="D15" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="E15" s="19" t="s">
         <v>40</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>41</v>
       </c>
       <c r="F15" s="20" t="s">
         <v>6</v>
@@ -1121,16 +1121,16 @@
     </row>
     <row r="16" spans="2:8" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="19" t="s">
+      <c r="E16" s="19" t="s">
         <v>43</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>44</v>
       </c>
       <c r="F16" s="20" t="s">
         <v>6</v>
@@ -1142,16 +1142,16 @@
     </row>
     <row r="17" spans="2:8" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="D17" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="E17" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>48</v>
       </c>
       <c r="F17" s="20" t="s">
         <v>6</v>
@@ -1163,22 +1163,22 @@
     </row>
     <row r="18" spans="2:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="23" t="s">
         <v>49</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="23" t="s">
-        <v>52</v>
       </c>
       <c r="H18" s="25"/>
     </row>
@@ -1189,18 +1189,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1421,18 +1421,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65FF626D-9FAF-46DB-862C-9BF32D1B1C2C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BD6D2F6-9AC3-4908-A36C-E9D9CCF4DE35}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BD6D2F6-9AC3-4908-A36C-E9D9CCF4DE35}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65FF626D-9FAF-46DB-862C-9BF32D1B1C2C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>